<commit_message>
update insert shipmnent id
</commit_message>
<xml_diff>
--- a/wwwroot/uploads/packinglist.xlsx
+++ b/wwwroot/uploads/packinglist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vincent_Pham\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6CB61A98-6C89-4667-9ABD-FE565E9E01A4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAA601FB-718E-4B3B-B40C-84586A7CB9B0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -141,18 +141,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -167,7 +161,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -176,10 +170,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -501,7 +491,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2:F3"/>
+      <selection pane="bottomLeft" activeCell="J1" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -690,73 +680,73 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="8" customFormat="1">
-      <c r="A6" s="6">
+    <row r="6" spans="1:11" s="2" customFormat="1">
+      <c r="A6" s="3">
         <v>336909</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="3">
         <v>1960027</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="3">
         <v>4504254060</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="3">
         <v>1088494</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="4">
         <v>1185</v>
       </c>
-      <c r="G6" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" s="6" t="s">
+      <c r="G6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="I6" s="7">
+      <c r="I6" s="4">
         <v>5000</v>
       </c>
-      <c r="J6" s="6">
-        <v>25</v>
-      </c>
-      <c r="K6" s="6">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" s="9" customFormat="1">
-      <c r="A7" s="6">
+      <c r="J6" s="3">
+        <v>25</v>
+      </c>
+      <c r="K6" s="3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="3">
         <v>336909</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="3">
         <v>1960027</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="3">
         <v>4504214556</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="3">
         <v>1088494</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="4">
         <v>1700</v>
       </c>
-      <c r="G7" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" s="6" t="s">
+      <c r="G7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="I7" s="7">
+      <c r="I7" s="4">
         <v>5000</v>
       </c>
-      <c r="J7" s="6">
-        <v>25</v>
-      </c>
-      <c r="K7" s="6">
+      <c r="J7" s="3">
+        <v>25</v>
+      </c>
+      <c r="K7" s="3">
         <v>22</v>
       </c>
     </row>

</xml_diff>